<commit_message>
More examples and added save to png mode
</commit_message>
<xml_diff>
--- a/Arkusze/Doktorat_obliczenia_EU-28_2007.xlsx
+++ b/Arkusze/Doktorat_obliczenia_EU-28_2007.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="130" documentId="13_ncr:1_{896BCC7E-4B88-4BD6-9EEE-69DADFE452C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{63D9E601-3AD8-4FA0-8CDC-717E10613B5C}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="60" windowWidth="15195" windowHeight="9210" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32760" yWindow="60" windowWidth="15195" windowHeight="9210" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dane " sheetId="1" r:id="rId1"/>
@@ -17209,7 +17209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AD92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -17431,19 +17431,19 @@
         <v>166.80385803767996</v>
       </c>
       <c r="W2" s="9">
-        <f>((B2-$B$30)^2+(C2-$C$30)^2+(D2-$D$30)^2+(E2-$E$30)^2+(F2-$F$30)^2+(G2-$G$30)^2+(H2-$H$30)^2+(I2-$I$30)^2+(J2-$J$30)^2+(K2-$K$30)^2+(L2-$L$30)^2+(M2-$M$30)^2+(N2-$N$30)^2+(O2-$O$30)^2+(P2-$P$30)^2+(Q2-$Q$30)^2+(R2-$R$30)^2+(S2-$S$30)^2+(T2-$T$30)^2+(U2-$U$30)^2+(V2-$V$30)^2)^(0.5)</f>
+        <f t="shared" ref="W2:W29" si="1">((B2-$B$30)^2+(C2-$C$30)^2+(D2-$D$30)^2+(E2-$E$30)^2+(F2-$F$30)^2+(G2-$G$30)^2+(H2-$H$30)^2+(I2-$I$30)^2+(J2-$J$30)^2+(K2-$K$30)^2+(L2-$L$30)^2+(M2-$M$30)^2+(N2-$N$30)^2+(O2-$O$30)^2+(P2-$P$30)^2+(Q2-$Q$30)^2+(R2-$R$30)^2+(S2-$S$30)^2+(T2-$T$30)^2+(U2-$U$30)^2+(V2-$V$30)^2)^(0.5)</f>
         <v>8634.6781258894953</v>
       </c>
       <c r="X2" s="9">
-        <f>1-(W2/$AD$3)</f>
+        <f t="shared" ref="X2:X29" si="2">1-(W2/$AD$3)</f>
         <v>0.34589823555157595</v>
       </c>
       <c r="Y2" t="str">
-        <f t="shared" ref="Y2:Y29" si="1">A2</f>
+        <f t="shared" ref="Y2:Y29" si="3">A2</f>
         <v>Austria</v>
       </c>
       <c r="Z2" s="10">
-        <f t="shared" ref="Z2:Z29" si="2">X2</f>
+        <f t="shared" ref="Z2:Z29" si="4">X2</f>
         <v>0.34589823555157595</v>
       </c>
       <c r="AA2" s="13">
@@ -17552,19 +17552,19 @@
         <v>76.7</v>
       </c>
       <c r="W3" s="9">
-        <f>((B3-$B$30)^2+(C3-$C$30)^2+(D3-$D$30)^2+(E3-$E$30)^2+(F3-$F$30)^2+(G3-$G$30)^2+(H3-$H$30)^2+(I3-$I$30)^2+(J3-$J$30)^2+(K3-$K$30)^2+(L3-$L$30)^2+(M3-$M$30)^2+(N3-$N$30)^2+(O3-$O$30)^2+(P3-$P$30)^2+(Q3-$Q$30)^2+(R3-$R$30)^2+(S3-$S$30)^2+(T3-$T$30)^2+(U3-$U$30)^2+(V3-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>8926.1795768087031</v>
       </c>
       <c r="X3" s="9">
-        <f>1-(W3/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.32381616015679837</v>
       </c>
       <c r="Y3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Belgia</v>
       </c>
       <c r="Z3" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.32381616015679837</v>
       </c>
       <c r="AA3" s="13">
@@ -17674,19 +17674,19 @@
         <v>33.18</v>
       </c>
       <c r="W4" s="9">
-        <f>((B4-$B$30)^2+(C4-$C$30)^2+(D4-$D$30)^2+(E4-$E$30)^2+(F4-$F$30)^2+(G4-$G$30)^2+(H4-$H$30)^2+(I4-$I$30)^2+(J4-$J$30)^2+(K4-$K$30)^2+(L4-$L$30)^2+(M4-$M$30)^2+(N4-$N$30)^2+(O4-$O$30)^2+(P4-$P$30)^2+(Q4-$Q$30)^2+(R4-$R$30)^2+(S4-$S$30)^2+(T4-$T$30)^2+(U4-$U$30)^2+(V4-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>10586.847407012154</v>
       </c>
       <c r="X4" s="9">
-        <f>1-(W4/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.19801578380670548</v>
       </c>
       <c r="Y4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Bułgaria</v>
       </c>
       <c r="Z4" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.19801578380670548</v>
       </c>
       <c r="AA4" s="13">
@@ -17793,19 +17793,19 @@
         <v>48.333333333333336</v>
       </c>
       <c r="W5" s="9">
-        <f>((B5-$B$30)^2+(C5-$C$30)^2+(D5-$D$30)^2+(E5-$E$30)^2+(F5-$F$30)^2+(G5-$G$30)^2+(H5-$H$30)^2+(I5-$I$30)^2+(J5-$J$30)^2+(K5-$K$30)^2+(L5-$L$30)^2+(M5-$M$30)^2+(N5-$N$30)^2+(O5-$O$30)^2+(P5-$P$30)^2+(Q5-$Q$30)^2+(R5-$R$30)^2+(S5-$S$30)^2+(T5-$T$30)^2+(U5-$U$30)^2+(V5-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>9625.0277696072153</v>
       </c>
       <c r="X5" s="9">
-        <f>1-(W5/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.27087639455968648</v>
       </c>
       <c r="Y5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Chorwacja</v>
       </c>
       <c r="Z5" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.27087639455968648</v>
       </c>
       <c r="AA5" s="13">
@@ -17912,19 +17912,19 @@
         <v>144.90352633826882</v>
       </c>
       <c r="W6" s="9">
-        <f>((B6-$B$30)^2+(C6-$C$30)^2+(D6-$D$30)^2+(E6-$E$30)^2+(F6-$F$30)^2+(G6-$G$30)^2+(H6-$H$30)^2+(I6-$I$30)^2+(J6-$J$30)^2+(K6-$K$30)^2+(L6-$L$30)^2+(M6-$M$30)^2+(N6-$N$30)^2+(O6-$O$30)^2+(P6-$P$30)^2+(Q6-$Q$30)^2+(R6-$R$30)^2+(S6-$S$30)^2+(T6-$T$30)^2+(U6-$U$30)^2+(V6-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>8492.1449980843809</v>
       </c>
       <c r="X6" s="9">
-        <f>1-(W6/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.35669553094932127</v>
       </c>
       <c r="Y6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Cypr</v>
       </c>
       <c r="Z6" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.35669553094932127</v>
       </c>
       <c r="AA6" s="13">
@@ -18031,19 +18031,19 @@
         <v>106.25</v>
       </c>
       <c r="W7" s="9">
-        <f>((B7-$B$30)^2+(C7-$C$30)^2+(D7-$D$30)^2+(E7-$E$30)^2+(F7-$F$30)^2+(G7-$G$30)^2+(H7-$H$30)^2+(I7-$I$30)^2+(J7-$J$30)^2+(K7-$K$30)^2+(L7-$L$30)^2+(M7-$M$30)^2+(N7-$N$30)^2+(O7-$O$30)^2+(P7-$P$30)^2+(Q7-$Q$30)^2+(R7-$R$30)^2+(S7-$S$30)^2+(T7-$T$30)^2+(U7-$U$30)^2+(V7-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>7562.7979571808883</v>
       </c>
       <c r="X7" s="9">
-        <f>1-(W7/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.42709624888891151</v>
       </c>
       <c r="Y7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Czechy</v>
       </c>
       <c r="Z7" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.42709624888891151</v>
       </c>
       <c r="AA7" s="13">
@@ -18150,19 +18150,19 @@
         <v>68.575000000000003</v>
       </c>
       <c r="W8" s="9">
-        <f>((B8-$B$30)^2+(C8-$C$30)^2+(D8-$D$30)^2+(E8-$E$30)^2+(F8-$F$30)^2+(G8-$G$30)^2+(H8-$H$30)^2+(I8-$I$30)^2+(J8-$J$30)^2+(K8-$K$30)^2+(L8-$L$30)^2+(M8-$M$30)^2+(N8-$N$30)^2+(O8-$O$30)^2+(P8-$P$30)^2+(Q8-$Q$30)^2+(R8-$R$30)^2+(S8-$S$30)^2+(T8-$T$30)^2+(U8-$U$30)^2+(V8-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>6710.3820660726115</v>
       </c>
       <c r="X8" s="9">
-        <f>1-(W8/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.49166921041553036</v>
       </c>
       <c r="Y8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Dania</v>
       </c>
       <c r="Z8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.49166921041553036</v>
       </c>
       <c r="AA8" s="13">
@@ -18269,19 +18269,19 @@
         <v>28.25</v>
       </c>
       <c r="W9" s="9">
-        <f>((B9-$B$30)^2+(C9-$C$30)^2+(D9-$D$30)^2+(E9-$E$30)^2+(F9-$F$30)^2+(G9-$G$30)^2+(H9-$H$30)^2+(I9-$I$30)^2+(J9-$J$30)^2+(K9-$K$30)^2+(L9-$L$30)^2+(M9-$M$30)^2+(N9-$N$30)^2+(O9-$O$30)^2+(P9-$P$30)^2+(Q9-$Q$30)^2+(R9-$R$30)^2+(S9-$S$30)^2+(T9-$T$30)^2+(U9-$U$30)^2+(V9-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>8620.333347376336</v>
       </c>
       <c r="X9" s="9">
-        <f>1-(W9/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.34698489388432219</v>
       </c>
       <c r="Y9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Estonia</v>
       </c>
       <c r="Z9" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.34698489388432219</v>
       </c>
       <c r="AA9" s="13">
@@ -18388,19 +18388,19 @@
         <v>132.69999999999999</v>
       </c>
       <c r="W10" s="9">
-        <f>((B10-$B$30)^2+(C10-$C$30)^2+(D10-$D$30)^2+(E10-$E$30)^2+(F10-$F$30)^2+(G10-$G$30)^2+(H10-$H$30)^2+(I10-$I$30)^2+(J10-$J$30)^2+(K10-$K$30)^2+(L10-$L$30)^2+(M10-$M$30)^2+(N10-$N$30)^2+(O10-$O$30)^2+(P10-$P$30)^2+(Q10-$Q$30)^2+(R10-$R$30)^2+(S10-$S$30)^2+(T10-$T$30)^2+(U10-$U$30)^2+(V10-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>10471.467863390235</v>
       </c>
       <c r="X10" s="9">
-        <f>1-(W10/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.20675611691050333</v>
       </c>
       <c r="Y10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Finlandia</v>
       </c>
       <c r="Z10" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.20675611691050333</v>
       </c>
       <c r="AA10" s="13">
@@ -18507,19 +18507,19 @@
         <v>434.97499999999997</v>
       </c>
       <c r="W11" s="9">
-        <f>((B11-$B$30)^2+(C11-$C$30)^2+(D11-$D$30)^2+(E11-$E$30)^2+(F11-$F$30)^2+(G11-$G$30)^2+(H11-$H$30)^2+(I11-$I$30)^2+(J11-$J$30)^2+(K11-$K$30)^2+(L11-$L$30)^2+(M11-$M$30)^2+(N11-$N$30)^2+(O11-$O$30)^2+(P11-$P$30)^2+(Q11-$Q$30)^2+(R11-$R$30)^2+(S11-$S$30)^2+(T11-$T$30)^2+(U11-$U$30)^2+(V11-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>9389.2242445029369</v>
       </c>
       <c r="X11" s="9">
-        <f>1-(W11/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.28873919147986438</v>
       </c>
       <c r="Y11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Francja</v>
       </c>
       <c r="Z11" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.28873919147986438</v>
       </c>
       <c r="AA11" s="13">
@@ -18626,19 +18626,19 @@
         <v>145.53229055046864</v>
       </c>
       <c r="W12" s="9">
-        <f>((B12-$B$30)^2+(C12-$C$30)^2+(D12-$D$30)^2+(E12-$E$30)^2+(F12-$F$30)^2+(G12-$G$30)^2+(H12-$H$30)^2+(I12-$I$30)^2+(J12-$J$30)^2+(K12-$K$30)^2+(L12-$L$30)^2+(M12-$M$30)^2+(N12-$N$30)^2+(O12-$O$30)^2+(P12-$P$30)^2+(Q12-$Q$30)^2+(R12-$R$30)^2+(S12-$S$30)^2+(T12-$T$30)^2+(U12-$U$30)^2+(V12-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>7741.1450545365087</v>
       </c>
       <c r="X12" s="9">
-        <f>1-(W12/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.41358594203511101</v>
       </c>
       <c r="Y12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Grecja</v>
       </c>
       <c r="Z12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.41358594203511101</v>
       </c>
       <c r="AA12" s="13">
@@ -18745,19 +18745,19 @@
         <v>259.75</v>
       </c>
       <c r="W13" s="9">
-        <f>((B13-$B$30)^2+(C13-$C$30)^2+(D13-$D$30)^2+(E13-$E$30)^2+(F13-$F$30)^2+(G13-$G$30)^2+(H13-$H$30)^2+(I13-$I$30)^2+(J13-$J$30)^2+(K13-$K$30)^2+(L13-$L$30)^2+(M13-$M$30)^2+(N13-$N$30)^2+(O13-$O$30)^2+(P13-$P$30)^2+(Q13-$Q$30)^2+(R13-$R$30)^2+(S13-$S$30)^2+(T13-$T$30)^2+(U13-$U$30)^2+(V13-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>10790.801253349471</v>
       </c>
       <c r="X13" s="9">
-        <f>1-(W13/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.18256569188546912</v>
       </c>
       <c r="Y13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Hiszpania</v>
       </c>
       <c r="Z13" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.18256569188546912</v>
       </c>
       <c r="AA13" s="13">
@@ -18864,19 +18864,19 @@
         <v>130.75</v>
       </c>
       <c r="W14" s="9">
-        <f>((B14-$B$30)^2+(C14-$C$30)^2+(D14-$D$30)^2+(E14-$E$30)^2+(F14-$F$30)^2+(G14-$G$30)^2+(H14-$H$30)^2+(I14-$I$30)^2+(J14-$J$30)^2+(K14-$K$30)^2+(L14-$L$30)^2+(M14-$M$30)^2+(N14-$N$30)^2+(O14-$O$30)^2+(P14-$P$30)^2+(Q14-$Q$30)^2+(R14-$R$30)^2+(S14-$S$30)^2+(T14-$T$30)^2+(U14-$U$30)^2+(V14-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>9424.3961343217561</v>
       </c>
       <c r="X14" s="9">
-        <f>1-(W14/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.28607481941479618</v>
       </c>
       <c r="Y14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Holandia</v>
       </c>
       <c r="Z14" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.28607481941479618</v>
       </c>
       <c r="AA14" s="13">
@@ -18983,19 +18983,19 @@
         <v>21.266666666666666</v>
       </c>
       <c r="W15" s="9">
-        <f>((B15-$B$30)^2+(C15-$C$30)^2+(D15-$D$30)^2+(E15-$E$30)^2+(F15-$F$30)^2+(G15-$G$30)^2+(H15-$H$30)^2+(I15-$I$30)^2+(J15-$J$30)^2+(K15-$K$30)^2+(L15-$L$30)^2+(M15-$M$30)^2+(N15-$N$30)^2+(O15-$O$30)^2+(P15-$P$30)^2+(Q15-$Q$30)^2+(R15-$R$30)^2+(S15-$S$30)^2+(T15-$T$30)^2+(U15-$U$30)^2+(V15-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>10012.995492200147</v>
       </c>
       <c r="X15" s="9">
-        <f>1-(W15/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.24148672094392198</v>
       </c>
       <c r="Y15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Irlandia</v>
       </c>
       <c r="Z15" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.24148672094392198</v>
       </c>
       <c r="AA15" s="13">
@@ -19102,19 +19102,19 @@
         <v>36.933333333333337</v>
       </c>
       <c r="W16" s="9">
-        <f>((B16-$B$30)^2+(C16-$C$30)^2+(D16-$D$30)^2+(E16-$E$30)^2+(F16-$F$30)^2+(G16-$G$30)^2+(H16-$H$30)^2+(I16-$I$30)^2+(J16-$J$30)^2+(K16-$K$30)^2+(L16-$L$30)^2+(M16-$M$30)^2+(N16-$N$30)^2+(O16-$O$30)^2+(P16-$P$30)^2+(Q16-$Q$30)^2+(R16-$R$30)^2+(S16-$S$30)^2+(T16-$T$30)^2+(U16-$U$30)^2+(V16-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>10653.39871711112</v>
       </c>
       <c r="X16" s="9">
-        <f>1-(W16/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.19297433017897059</v>
       </c>
       <c r="Y16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Litwa</v>
       </c>
       <c r="Z16" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.19297433017897059</v>
       </c>
       <c r="AA16" s="13">
@@ -19221,19 +19221,19 @@
         <v>9.64</v>
       </c>
       <c r="W17" s="9">
-        <f>((B17-$B$30)^2+(C17-$C$30)^2+(D17-$D$30)^2+(E17-$E$30)^2+(F17-$F$30)^2+(G17-$G$30)^2+(H17-$H$30)^2+(I17-$I$30)^2+(J17-$J$30)^2+(K17-$K$30)^2+(L17-$L$30)^2+(M17-$M$30)^2+(N17-$N$30)^2+(O17-$O$30)^2+(P17-$P$30)^2+(Q17-$Q$30)^2+(R17-$R$30)^2+(S17-$S$30)^2+(T17-$T$30)^2+(U17-$U$30)^2+(V17-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>10480.025657361763</v>
       </c>
       <c r="X17" s="9">
-        <f>1-(W17/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.20610783934242827</v>
       </c>
       <c r="Y17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Luksemburg</v>
       </c>
       <c r="Z17" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.20610783934242827</v>
       </c>
       <c r="AA17" s="13">
@@ -19340,19 +19340,19 @@
         <v>27.9</v>
       </c>
       <c r="W18" s="9">
-        <f>((B18-$B$30)^2+(C18-$C$30)^2+(D18-$D$30)^2+(E18-$E$30)^2+(F18-$F$30)^2+(G18-$G$30)^2+(H18-$H$30)^2+(I18-$I$30)^2+(J18-$J$30)^2+(K18-$K$30)^2+(L18-$L$30)^2+(M18-$M$30)^2+(N18-$N$30)^2+(O18-$O$30)^2+(P18-$P$30)^2+(Q18-$Q$30)^2+(R18-$R$30)^2+(S18-$S$30)^2+(T18-$T$30)^2+(U18-$U$30)^2+(V18-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>465.23439389380349</v>
       </c>
       <c r="X18" s="9">
-        <f>1-(W18/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.96475715324979971</v>
       </c>
       <c r="Y18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Łotwa</v>
       </c>
       <c r="Z18" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.96475715324979971</v>
       </c>
       <c r="AA18" s="13">
@@ -19459,19 +19459,19 @@
         <v>143.91419305977459</v>
       </c>
       <c r="W19" s="9">
-        <f>((B19-$B$30)^2+(C19-$C$30)^2+(D19-$D$30)^2+(E19-$E$30)^2+(F19-$F$30)^2+(G19-$G$30)^2+(H19-$H$30)^2+(I19-$I$30)^2+(J19-$J$30)^2+(K19-$K$30)^2+(L19-$L$30)^2+(M19-$M$30)^2+(N19-$N$30)^2+(O19-$O$30)^2+(P19-$P$30)^2+(Q19-$Q$30)^2+(R19-$R$30)^2+(S19-$S$30)^2+(T19-$T$30)^2+(U19-$U$30)^2+(V19-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>10344.837094789393</v>
       </c>
       <c r="X19" s="9">
-        <f>1-(W19/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.21634876274717008</v>
       </c>
       <c r="Y19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Malta</v>
       </c>
       <c r="Z19" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.21634876274717008</v>
       </c>
       <c r="AA19" s="13">
@@ -19578,19 +19578,19 @@
         <v>101.7</v>
       </c>
       <c r="W20" s="9">
-        <f>((B20-$B$30)^2+(C20-$C$30)^2+(D20-$D$30)^2+(E20-$E$30)^2+(F20-$F$30)^2+(G20-$G$30)^2+(H20-$H$30)^2+(I20-$I$30)^2+(J20-$J$30)^2+(K20-$K$30)^2+(L20-$L$30)^2+(M20-$M$30)^2+(N20-$N$30)^2+(O20-$O$30)^2+(P20-$P$30)^2+(Q20-$Q$30)^2+(R20-$R$30)^2+(S20-$S$30)^2+(T20-$T$30)^2+(U20-$U$30)^2+(V20-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>10547.995447456353</v>
       </c>
       <c r="X20" s="9">
-        <f>1-(W20/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.20095893176511426</v>
       </c>
       <c r="Y20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Niemcy</v>
       </c>
       <c r="Z20" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.20095893176511426</v>
       </c>
       <c r="AA20" s="13">
@@ -19697,19 +19697,19 @@
         <v>329.4</v>
       </c>
       <c r="W21" s="9">
-        <f>((B21-$B$30)^2+(C21-$C$30)^2+(D21-$D$30)^2+(E21-$E$30)^2+(F21-$F$30)^2+(G21-$G$30)^2+(H21-$H$30)^2+(I21-$I$30)^2+(J21-$J$30)^2+(K21-$K$30)^2+(L21-$L$30)^2+(M21-$M$30)^2+(N21-$N$30)^2+(O21-$O$30)^2+(P21-$P$30)^2+(Q21-$Q$30)^2+(R21-$R$30)^2+(S21-$S$30)^2+(T21-$T$30)^2+(U21-$U$30)^2+(V21-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>6797.9507725878584</v>
       </c>
       <c r="X21" s="9">
-        <f>1-(W21/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.48503562840969394</v>
       </c>
       <c r="Y21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Polska</v>
       </c>
       <c r="Z21" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.48503562840969394</v>
       </c>
       <c r="AA21" s="13">
@@ -19816,19 +19816,19 @@
         <v>95.699999999999989</v>
       </c>
       <c r="W22" s="9">
-        <f>((B22-$B$30)^2+(C22-$C$30)^2+(D22-$D$30)^2+(E22-$E$30)^2+(F22-$F$30)^2+(G22-$G$30)^2+(H22-$H$30)^2+(I22-$I$30)^2+(J22-$J$30)^2+(K22-$K$30)^2+(L22-$L$30)^2+(M22-$M$30)^2+(N22-$N$30)^2+(O22-$O$30)^2+(P22-$P$30)^2+(Q22-$Q$30)^2+(R22-$R$30)^2+(S22-$S$30)^2+(T22-$T$30)^2+(U22-$U$30)^2+(V22-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>6630.0619897127026</v>
       </c>
       <c r="X22" s="9">
-        <f>1-(W22/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.49775368778708684</v>
       </c>
       <c r="Y22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Portugalia</v>
       </c>
       <c r="Z22" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.49775368778708684</v>
       </c>
       <c r="AA22" s="13">
@@ -19935,19 +19935,19 @@
         <v>239.1</v>
       </c>
       <c r="W23" s="9">
-        <f>((B23-$B$30)^2+(C23-$C$30)^2+(D23-$D$30)^2+(E23-$E$30)^2+(F23-$F$30)^2+(G23-$G$30)^2+(H23-$H$30)^2+(I23-$I$30)^2+(J23-$J$30)^2+(K23-$K$30)^2+(L23-$L$30)^2+(M23-$M$30)^2+(N23-$N$30)^2+(O23-$O$30)^2+(P23-$P$30)^2+(Q23-$Q$30)^2+(R23-$R$30)^2+(S23-$S$30)^2+(T23-$T$30)^2+(U23-$U$30)^2+(V23-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>8087.2616146172577</v>
       </c>
       <c r="X23" s="9">
-        <f>1-(W23/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.38736661464931865</v>
       </c>
       <c r="Y23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Rumunia</v>
       </c>
       <c r="Z23" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.38736661464931865</v>
       </c>
       <c r="AA23" s="13">
@@ -20054,19 +20054,19 @@
         <v>144.01113543840199</v>
       </c>
       <c r="W24" s="9">
-        <f>((B24-$B$30)^2+(C24-$C$30)^2+(D24-$D$30)^2+(E24-$E$30)^2+(F24-$F$30)^2+(G24-$G$30)^2+(H24-$H$30)^2+(I24-$I$30)^2+(J24-$J$30)^2+(K24-$K$30)^2+(L24-$L$30)^2+(M24-$M$30)^2+(N24-$N$30)^2+(O24-$O$30)^2+(P24-$P$30)^2+(Q24-$Q$30)^2+(R24-$R$30)^2+(S24-$S$30)^2+(T24-$T$30)^2+(U24-$U$30)^2+(V24-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>10372.9420719149</v>
       </c>
       <c r="X24" s="9">
-        <f>1-(W24/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.21421972969468628</v>
       </c>
       <c r="Y24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Słowacja</v>
       </c>
       <c r="Z24" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.21421972969468628</v>
       </c>
       <c r="AA24" s="13">
@@ -20173,19 +20173,19 @@
         <v>23.599999999999998</v>
       </c>
       <c r="W25" s="9">
-        <f>((B25-$B$30)^2+(C25-$C$30)^2+(D25-$D$30)^2+(E25-$E$30)^2+(F25-$F$30)^2+(G25-$G$30)^2+(H25-$H$30)^2+(I25-$I$30)^2+(J25-$J$30)^2+(K25-$K$30)^2+(L25-$L$30)^2+(M25-$M$30)^2+(N25-$N$30)^2+(O25-$O$30)^2+(P25-$P$30)^2+(Q25-$Q$30)^2+(R25-$R$30)^2+(S25-$S$30)^2+(T25-$T$30)^2+(U25-$U$30)^2+(V25-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>10496.750592512426</v>
       </c>
       <c r="X25" s="9">
-        <f>1-(W25/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.20484087728167311</v>
       </c>
       <c r="Y25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Słowenia</v>
       </c>
       <c r="Z25" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.20484087728167311</v>
       </c>
       <c r="AA25" s="13">
@@ -20292,19 +20292,19 @@
         <v>71.7</v>
       </c>
       <c r="W26" s="9">
-        <f>((B26-$B$30)^2+(C26-$C$30)^2+(D26-$D$30)^2+(E26-$E$30)^2+(F26-$F$30)^2+(G26-$G$30)^2+(H26-$H$30)^2+(I26-$I$30)^2+(J26-$J$30)^2+(K26-$K$30)^2+(L26-$L$30)^2+(M26-$M$30)^2+(N26-$N$30)^2+(O26-$O$30)^2+(P26-$P$30)^2+(Q26-$Q$30)^2+(R26-$R$30)^2+(S26-$S$30)^2+(T26-$T$30)^2+(U26-$U$30)^2+(V26-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>9300.1657653653801</v>
       </c>
       <c r="X26" s="9">
-        <f>1-(W26/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.29548562805730982</v>
       </c>
       <c r="Y26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Szwecja</v>
       </c>
       <c r="Z26" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.29548562805730982</v>
       </c>
       <c r="AA26" s="13">
@@ -20411,19 +20411,19 @@
         <v>144.12425003756678</v>
       </c>
       <c r="W27" s="9">
-        <f>((B27-$B$30)^2+(C27-$C$30)^2+(D27-$D$30)^2+(E27-$E$30)^2+(F27-$F$30)^2+(G27-$G$30)^2+(H27-$H$30)^2+(I27-$I$30)^2+(J27-$J$30)^2+(K27-$K$30)^2+(L27-$L$30)^2+(M27-$M$30)^2+(N27-$N$30)^2+(O27-$O$30)^2+(P27-$P$30)^2+(Q27-$Q$30)^2+(R27-$R$30)^2+(S27-$S$30)^2+(T27-$T$30)^2+(U27-$U$30)^2+(V27-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>10143.029155454027</v>
       </c>
       <c r="X27" s="9">
-        <f>1-(W27/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.23163629602570379</v>
       </c>
       <c r="Y27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Węgry</v>
       </c>
       <c r="Z27" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.23163629602570379</v>
       </c>
       <c r="AA27" s="13">
@@ -20530,19 +20530,19 @@
         <v>325.20000000000005</v>
       </c>
       <c r="W28" s="9">
-        <f>((B28-$B$30)^2+(C28-$C$30)^2+(D28-$D$30)^2+(E28-$E$30)^2+(F28-$F$30)^2+(G28-$G$30)^2+(H28-$H$30)^2+(I28-$I$30)^2+(J28-$J$30)^2+(K28-$K$30)^2+(L28-$L$30)^2+(M28-$M$30)^2+(N28-$N$30)^2+(O28-$O$30)^2+(P28-$P$30)^2+(Q28-$Q$30)^2+(R28-$R$30)^2+(S28-$S$30)^2+(T28-$T$30)^2+(U28-$U$30)^2+(V28-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>4849.1800712441027</v>
       </c>
       <c r="X28" s="9">
-        <f>1-(W28/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.63266062793716982</v>
       </c>
       <c r="Y28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Wielka Brytania</v>
       </c>
       <c r="Z28" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.63266062793716982</v>
       </c>
       <c r="AA28" s="13">
@@ -20649,19 +20649,19 @@
         <v>144.2523062613476</v>
       </c>
       <c r="W29" s="9">
-        <f>((B29-$B$30)^2+(C29-$C$30)^2+(D29-$D$30)^2+(E29-$E$30)^2+(F29-$F$30)^2+(G29-$G$30)^2+(H29-$H$30)^2+(I29-$I$30)^2+(J29-$J$30)^2+(K29-$K$30)^2+(L29-$L$30)^2+(M29-$M$30)^2+(N29-$N$30)^2+(O29-$O$30)^2+(P29-$P$30)^2+(Q29-$Q$30)^2+(R29-$R$30)^2+(S29-$S$30)^2+(T29-$T$30)^2+(U29-$U$30)^2+(V29-$V$30)^2)^(0.5)</f>
+        <f t="shared" si="1"/>
         <v>8983.7754840000289</v>
       </c>
       <c r="X29" s="9">
-        <f>1-(W29/$AD$3)</f>
+        <f t="shared" si="2"/>
         <v>0.319453104120477</v>
       </c>
       <c r="Y29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Włochy</v>
       </c>
       <c r="Z29" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.319453104120477</v>
       </c>
       <c r="AA29" s="13">
@@ -20695,63 +20695,63 @@
         <v>1</v>
       </c>
       <c r="E30" s="17">
-        <f t="shared" ref="E30:K30" si="3">MIN(E2:E29)</f>
+        <f t="shared" ref="E30:K30" si="5">MIN(E2:E29)</f>
         <v>-24</v>
       </c>
       <c r="F30" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.9</v>
       </c>
       <c r="G30" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.1</v>
       </c>
       <c r="H30" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9.8571428571428577</v>
       </c>
       <c r="I30" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8.8000000000000007</v>
       </c>
       <c r="J30" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-7</v>
       </c>
       <c r="K30" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>294</v>
       </c>
       <c r="L30" s="8">
-        <f t="shared" ref="L30:S30" si="4">MAX(L2:L29)</f>
+        <f t="shared" ref="L30:S30" si="6">MAX(L2:L29)</f>
         <v>44.2</v>
       </c>
       <c r="M30" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>178.4</v>
       </c>
       <c r="N30" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="O30" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10947</v>
       </c>
       <c r="P30" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.02</v>
       </c>
       <c r="Q30" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.74</v>
       </c>
       <c r="R30" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>78.03</v>
       </c>
       <c r="S30" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.35</v>
       </c>
       <c r="T30" s="17">
@@ -34626,7 +34626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74E5D8A-E04B-4C6F-99EE-C1B478FE0620}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>